<commit_message>
Updated the python code to handle the file does not exist error
</commit_message>
<xml_diff>
--- a/Daily Sales Dashboard(1).xlsx
+++ b/Daily Sales Dashboard(1).xlsx
@@ -156,15 +156,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="table2" displayName="table2" ref="A1:F22" headerRowCount="1">
-  <autoFilter ref="A1:F22"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Dashboard Name"/>
-    <tableColumn id="2" name="Connection Name"/>
-    <tableColumn id="3" name="Connection ID"/>
-    <tableColumn id="4" name="Data Source"/>
-    <tableColumn id="5" name="Data Source Type"/>
-    <tableColumn id="6" name="Table Name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="table2" displayName="table2" ref="A1:A1" headerRowCount="1">
+  <autoFilter ref="A1:A1"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="None"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -209,8 +204,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="table6" displayName="table6" ref="A1:C36" headerRowCount="1">
-  <autoFilter ref="A1:C36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="table6" displayName="table6" ref="A1:C2" headerRowCount="1">
+  <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Dashboard Name"/>
     <tableColumn id="2" name="Table Name"/>
@@ -559,727 +554,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="31.2" customWidth="1" min="1" max="1"/>
-    <col width="20.4" customWidth="1" min="2" max="2"/>
-    <col width="25.2" customWidth="1" min="3" max="3"/>
-    <col width="25.2" customWidth="1" min="4" max="4"/>
-    <col width="25.2" customWidth="1" min="5" max="5"/>
-    <col width="61.2" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Dashboard Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Connection Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Connection ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Data Source</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Data Source Type</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Table Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\ESDOV0001-ZE_ESDOV0001_C000_00001</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\MST_SLSMAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\SET_REF</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\vQlikSense_Product</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>AOP 2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>DailyDashboard\MonthAndWeekSalesAndAOPLast2Months</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>Excel\SalesModel\LE</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>Excel\SalesModel\LE</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\MST_PRDUOM</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>CDCKeyAccount\IsandoOrderMan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>CDCKeyAccount\ParowOrderMan</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>CDCKeyAccount\PinetownOrderMan</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>CDCKeyAccount\InvoicedQty</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>CloseToExpiry\LeadDayByAddressAndType</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F19" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\ESDOV0001-ZE_ESDOV0001_C000_00001</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F20" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\MST_SLSMAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>MasterData\SET_REF</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>QSData</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>cwwpvt_qlikviewdev3</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>DC MAP - Daily Sales</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3959,7 +3241,7 @@
     <col width="27.6" customWidth="1" min="3" max="3"/>
     <col width="13.2" customWidth="1" min="4" max="4"/>
     <col width="1880.4" customWidth="1" min="5" max="5"/>
-    <col width="987.5999999999999" customWidth="1" min="6" max="6"/>
+    <col width="1053.6" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4056,28 +3338,25 @@
         <is>
           <t xml:space="preserve">
 SWITCH(
- VALUELIST('AOP(T)','Delivery Orders(T)','Variance (Orders vs AOP)','Invoiced Volumes(T)','Variance (Invoice vs AOP)'),
- 'AOP(T)', DIVIDE(
-    SUMX(
-        FILTER(
-            ALL('Table'),
-            'Table'[MONTHNO] = MAX('Table'[MONTHNO])
-                &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports"
+    VALUELIST('AOP(T)','Delivery Orders(T)','Variance (Orders vs AOP)','Invoiced Volumes(T)','Variance (Invoice vs AOP)'),
+    'AOP(T)', 
+        DIVIDE(
+            SUMX(
+                FILTER(ALL('Table'), 
+                    AND('Table'[MONTHNO] = MAX('Table'[MONTHNO]),
+                        'Table'[CATEGORY] &lt;&gt; "Exports")
+                ), 
+                'Table'[AOPVol]
+            ), 
+            NETWORKDAYS.INTL(
+                STARTOFMONTH(MAKEDATE(MAX('Table'[vMaxYear]), MAX('Table'[vMaxMonth]))), 
+                ENDOFMONTH(MAKEDATE(MAX('Table'[vMaxYear]), MAX('Table'[vMaxMonth]))), 
+                MAX('Table'[vWorkingDays])
+            )
         ),
-        'Table'[AOPVol]
-    ),
-    NETWORKDAYS.INTL(
-        STARTOFMONTH('Table'[Makedate]),
-        ENDOFMONTH('Table'[Makedate]),
-        $(vWorkingDays)
-    )
-),
- 'Delivery Orders(T)', DIVIDE(
-    SUMX(
-        FILTER(
-            ALL('Table'),
-            'Table'[TRANS_DATE] = MAX('Table'[TRANS_DATE])
-                &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "</t>
+    'Delivery Orders(T)', 
+        DIVIDE(
+           </t>
         </is>
       </c>
     </row>
@@ -4725,7 +4004,7 @@
       <c r="F21" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-FORMAT(DIVIDE(SUMX(FILTER(ALL(TableName), TableName[TRANS_DATE] &lt; MAX(TableName[TRANS_DATE]) &amp;&amp; TableName[WEEK] = MAX(TableName[WEEK]) &amp;&amp; TableName[WEEKDAY] = "Fri"), TableName[MonthWeight] + TableName[Weight]), 1000), "# ##0")</t>
+FORMAT(DIVIDE(SUMX(FILTER(ALL(TableName), TableName[TRANS_DATE] &lt; MAX(TableName[TRANS_DATE]) &amp;&amp; TableName[WEEK] = MAX(TableName[WEEK]) &amp;&amp; TableName[WEEKDAY] = "Fri"), [MonthWeight] + [Weight]), 1000), "# ##0")</t>
         </is>
       </c>
     </row>
@@ -4758,7 +4037,7 @@
       <c r="F22" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-FORMAT(DIVIDE(SUMX(FILTER(ALL(TableName), TableName[TRANS_DATE] &lt; MAX(TableName[TRANS_DATE]) &amp;&amp; TableName[WEEK] = MAX(TableName[WEEK]) &amp;&amp; TableName[WEEKDAY] = "Sat"), [MonthWeight] + [Weight]), 1000), "# ##0")</t>
+FORMAT(DIVIDE(SUMX(FILTER(ALL(TableName), TableName[TRANS_DATE] &lt; MAX(TableName[TRANS_DATE]) &amp;&amp; TableName[WEEK] = MAX(TableName[WEEK]) &amp;&amp; TableName[WEEKDAY] = "Sat"), TableName[MonthWeight] + TableName[Weight]), 1000), "# ##0")</t>
         </is>
       </c>
     </row>
@@ -5205,7 +4484,7 @@
       <c r="F35" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[AgeBucket] = "0-3 Days" &amp;&amp; 'Table'[ROUTE_LOCATION] = "HEILBRON" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Wholesale"), [KG's]), 1000), "# ##0") &amp; " T"</t>
+FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[AgeBucket] = "0-3 Days" &amp;&amp; 'Table'[ROUTE_LOCATION] = "HEILBRON" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Wholesale"), [KG's]), 1000), "# ##0 T")</t>
         </is>
       </c>
     </row>
@@ -5271,7 +4550,7 @@
       <c r="F37" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[AgeBucket] = "Greater than 5 Days", 'Table'[ROUTE_LOCATION] = "HEILBRON", NOT('Table'[CATEGORY] = "Wholesale")), [KG's]), 1000), "# ##0") &amp; " T"</t>
+FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[AgeBucket] = "Greater than 5 Days", 'Table'[ROUTE_LOCATION] = "HEILBRON", NOT('Table'[CATEGORY] = "Wholesale")), 'Table'[KG's]), 1000), "# ##0 T")</t>
         </is>
       </c>
     </row>
@@ -5370,7 +4649,7 @@
       <c r="F40" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-=FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &lt; $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek) &amp;&amp; 'Table'[WEEKDAY] = "Wed" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Table'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), 'Table'[MonthWeight]) + SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &gt;= $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek) &amp;&amp; 'Table'[WEEKDAY] = "Wed" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Table'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), 'Table'[Weight]), 1000), "# ##0")</t>
+=FORMAT(SUMX(FILTER(ALL(TableName), 'TableName'[TRANS_DATE] &lt; $(vPrevDate) &amp;&amp; 'TableName'[WEEK] = $(vMaxWeek) &amp;&amp; 'TableName'[WEEKDAY] = "Wed" &amp;&amp; 'TableName'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'TableName'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), 'TableName'[MonthWeight]) + SUMX(FILTER(ALL(TableName), 'TableName'[TRANS_DATE] &gt;= $(vPrevDate) &amp;&amp; 'TableName'[WEEK] = $(vMaxWeek) &amp;&amp; 'TableName'[WEEKDAY] = "Wed" &amp;&amp; 'TableName'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'TableName'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), 'TableName'[Weight])/1000, "# ##0")</t>
         </is>
       </c>
     </row>
@@ -5436,7 +4715,7 @@
       <c r="F42" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-=FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &lt; $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek) &amp;&amp; 'Table'[WEEKDAY] = "Fri" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Table'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), [MonthWeight] + SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &gt;= $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek) &amp;&amp; 'Table'[WEEKDAY] = "Fri" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Table'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), [Weight])), "# ##0")</t>
+=FORMAT(DIVIDE(SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &lt; $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek) &amp;&amp; 'Table'[WEEKDAY] = "Fri" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Table'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), 'Table'[MonthWeight]) + SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &gt;= $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek) &amp;&amp; 'Table'[WEEKDAY] = "Fri" &amp;&amp; 'Table'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Table'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"), 'Table'[Weight]), 1000), "# ##0")</t>
         </is>
       </c>
     </row>
@@ -5589,28 +4868,35 @@
       <c r="F46" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-SUMX (
-    FILTER (
-        ALL ( 'Date'[Date] ),
-        'Date'[Date] &lt; DATE ( YEAR ( vMaxYear ), MONTH ( vMaxMonth ), 1 )
-            || ( 'Date'[Date] &gt;= DATE ( YEAR ( vMaxYear ), MONTH ( vMaxMonth ), 1 )
-                &amp;&amp; 'Date'[Week] = vMaxWeek
-                &amp;&amp; 'Date'[Weekday] = "Tue"
-                &amp;&amp; 'Trans'[CATEGORY] &lt;&gt; "Exports"
-                &amp;&amp; 'Trans'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS" )
+SUMX(
+    FILTER(
+        ALL(TRANS_DATE),
+        TRANS_DATE &lt; DATE(vMaxYear, vMaxMonth, 1),
+        WEEK = vMaxWeek,
+        WEEKDAY = "Tue",
+        CATEGORY &lt;&gt; "Exports",
+        ITEM_PACKSIZE_GROUP &lt;&gt; "BALERS"
     ),
-    [MonthWeight] + [Weight]
-)
-/
-DIVIDE (
-    SUMX (
-        FILTER (
-            ALL ( 'Date' ),
-            'Date'[MonthNo] = vMaxMonth
-                &amp;&amp; 'Trans'[CATEGORY] &lt;&gt; "Exports"
-                &amp;&amp; 'Trans'[ITEM_PACKSIZE_GROUP] &lt;&gt; "BALERS"
-        ),
-        [AOPVol]</t>
+    [MonthWeight]
+) +
+SUMX(
+    FILTER(
+        ALL(TRANS_DATE),
+        TRANS_DATE &gt;= DATE(vMaxYear, vMaxMonth, 1),
+        WEEK = vMaxWeek,
+        WEEKDAY = "Tue",
+        CATEGORY &lt;&gt; "Exports",
+        ITEM_PACKSIZE_GROUP &lt;&gt; "BALERS"
+    ),
+    [Weight]
+) /
+(
+    SUMX(
+        FILTER(
+            ALL(MONTHNO),
+            MONTHNO = vMaxMonth,
+            CATEGORY &lt;&gt; "Exports",
+            ITEM_PACKSIZE_GROUP &lt;&gt; "B</t>
         </is>
       </c>
     </row>
@@ -5704,29 +4990,35 @@
       <c r="F48" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-SUMX (
-    FILTER (
-        ALL ( 'Date'[Date] ),
-        'Date'[Date] &lt; DATE ( YEAR ( vMaxYear ), MONTH ( vMaxMonth ), 1 )
-            || (
-                'Date'[Date] &gt;= DATE ( YEAR ( vMaxYear ), MONTH ( vMaxMonth ), 1 )
-                &amp;&amp; 'Date'[Week] = vMaxWeek
-                &amp;&amp; 'Date'[Weekday] = "Thu"
-                &amp;&amp; 'Data'[Category] &lt;&gt; "Exports"
-                &amp;&amp; 'Data'[Item_Packsize_Group] &lt;&gt; "BALERS"
-            )
+=DIVIDE(
+    SUMX(
+        FILTER(
+            ALL(Trans_Date),
+            Trans_Date &lt; DATE(vMaxYear, vMaxMonth, 1)
+            &amp;&amp; WEEK = vMaxWeek
+            &amp;&amp; WEEKDAY = "Thu"
+            &amp;&amp; CATEGORY &lt;&gt; "Exports"
+            &amp;&amp; ITEM_PACKSIZE_GROUP &lt;&gt; "BALERS"
+        ),
+        [MonthWeight]
+    ) + SUMX(
+        FILTER(
+            ALL(Trans_Date),
+            Trans_Date &gt;= DATE(vMaxYear, vMaxMonth, 1)
+            &amp;&amp; WEEK = vMaxWeek
+            &amp;&amp; WEEKDAY = "Thu"
+            &amp;&amp; CATEGORY &lt;&gt; "Exports"
+            &amp;&amp; ITEM_PACKSIZE_GROUP &lt;&gt; "BALERS"
+        ),
+        [Weight]
     ),
-    [MonthWeight] + [Weight]
-)
-/
-DIVIDE (
-    SUM ( 'Data'[AOPVol] ),
-    CALCULATE (
-        DISTINCTCOUNT ( 'Date'[Date] ),
-        FILTER (
-            ALL ( 'Date' ),
-            'Date'[Date] &gt;= DATE ( YEAR ( vMaxYear ), MONTH ( vMaxMonth ), 1 )
-                &amp;&amp; 'Date'</t>
+    DIVIDE(
+        SUMX(
+            FILTER(
+                ALL(MonthNo),
+                MonthNo = vMaxMonth
+                &amp;&amp; CATEGORY &lt;&gt; "Exports"
+                &amp;&amp; ITEM_PACK</t>
         </is>
       </c>
     </row>
@@ -5820,7 +5112,7 @@
       <c r="F50" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-= FORMAT (DIVIDE ( SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &lt; $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Mon", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [MonthWeight] ) + SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &gt;= $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Mon", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [Weight] ), 0, "# ##0" )</t>
+= FORMAT (DIVIDE ( SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &lt; $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Mon", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [MonthWeight] ) + SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &gt;= $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Mon", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [Weight] ), 1000, "# ##0" )</t>
         </is>
       </c>
     </row>
@@ -5853,7 +5145,7 @@
       <c r="F51" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-= FORMAT (DIVIDE ( SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &lt; vPrevDate &amp;&amp; 'Transactions'[WEEK] = vMaxWeek &amp;&amp; 'Transactions'[WEEKDAY] = "Tue" &amp;&amp; 'Transactions'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [MonthWeight] ) + SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &gt;= vPrevDate &amp;&amp; 'Transactions'[WEEK] = vMaxWeek &amp;&amp; 'Transactions'[WEEKDAY] = "Tue" &amp;&amp; 'Transactions'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [Weight] ), 0 ), "# ##0" )</t>
+= FORMAT (DIVIDE ( SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &lt; vPrevDate &amp;&amp; 'Transactions'[WEEK] = vMaxWeek &amp;&amp; 'Transactions'[WEEKDAY] = "Tue" &amp;&amp; 'Transactions'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), 'Transactions'[MonthWeight] ) + SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &gt;= vPrevDate &amp;&amp; 'Transactions'[WEEK] = vMaxWeek &amp;&amp; 'Transactions'[WEEKDAY] = "Tue" &amp;&amp; 'Transactions'[CATEGORY] &lt;&gt; "Exports" &amp;&amp; 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), 'Transactions'[Weight] ), 1000, "# ##0" )</t>
         </is>
       </c>
     </row>
@@ -5919,7 +5211,7 @@
       <c r="F53" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-= FORMAT (DIVIDE ( SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &lt; $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Thu", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [MonthWeight] ) + SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &gt;= $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Thu", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [Weight] ), 0 ), "# ##0" )</t>
+= FORMAT (DIVIDE ( SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &lt; $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Thu", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [MonthWeight] ) + SUMX ( FILTER ( ALL ( 'Transactions' ), 'Transactions'[TRANS_DATE] &gt;= $(vPrevDate), 'Transactions'[WEEK] = $(vMaxWeek), 'Transactions'[WEEKDAY] = "Thu", 'Transactions'[CATEGORY] &lt;&gt; "Exports", 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS" ), [Weight] ), 0, "# ##0" )</t>
         </is>
       </c>
     </row>
@@ -6118,6 +5410,62 @@
       <c r="F58" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
+SUMX (
+    FILTER ( 
+        ALL ( TRANS_DATE, WEEK, WEEKDAY, CATEGORY, ITEM_PACKSIZE_GROUP ),
+        TRANS_DATE &lt; DATE ( vMaxYear, vMaxMonth, 1 ) 
+            &amp;&amp; WEEK = vMaxWeek
+            &amp;&amp; WEEKDAY = "Tue"
+            &amp;&amp; CATEGORY &lt;&gt; "Exports" 
+            &amp;&amp; ITEM_PACKSIZE_GROUP = "BALERS"
+    ), 
+    [MonthWeight]
+) + 
+SUMX (
+    FILTER ( 
+        ALL ( TRANS_DATE, WEEK, WEEKDAY, CATEGORY, ITEM_PACKSIZE_GROUP ),
+        TRANS_DATE &gt;= DATE ( vMaxYear, vMaxMonth, 1 ) 
+            &amp;&amp; WEEK = vMaxWeek
+            &amp;&amp; WEEKDAY = "Tue"
+            &amp;&amp; CATEGORY &lt;&gt; "Exports" 
+            &amp;&amp; ITEM_PACKSIZE_GROUP = "BALERS"
+    ), 
+    [Weight]
+) 
+/ 
+DIVIDE (</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>Daily Sales Dashboard(1)</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>My new sheet (2)</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>qsSimpleKPI</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>Measure</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>['=\r\n(sum({&lt;TRANS_DATE={"&lt;$(vPrevDate)"}, WEEK={$(vMaxWeek)}, WEEKDAY = {\'Wed\'}, CATEGORY-={\'Exports\'}, ITEM_PACKSIZE_GROUP={\'BALERS\'}&gt;}MonthWeight)\n+ sum({&lt;TRANS_DATE={"&gt;=$(vPrevDate)"}, WEEK={$(vMaxWeek)}, WEEKDAY = {\'Wed\'}, CATEGORY-={\'Exports\'}, ITEM_PACKSIZE_GROUP={\'BALERS\'}&gt;}Weight))/\n(\n((sum({&lt;MONTHNO={$(vMaxMonth)}, CATEGORY-={\'Exports\'}, ITEM_PACKSIZE_GROUP={\'BALERS\'}&gt;} AOPVol)/\nNetWorkDays(monthstart(Makedate(vMaxYear,vMaxMonth)),MonthEnd(Makedate(vMaxYear,vMaxMonth)),$(vWorkingDays))))\n)']</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
 DIVIDE(
     ADD(
         SUMX(
@@ -6125,7 +5473,7 @@
                 ALL('Transactions'),
                 'Transactions'[TRANS_DATE] &lt; DATE(vMaxYear, vMaxMonth, 1)
                 &amp;&amp; 'Transactions'[WEEK] = vMaxWeek
-                &amp;&amp; 'Transactions'[WEEKDAY] = "Tue"
+                &amp;&amp; 'Transactions'[WEEKDAY] = "Wed"
                 &amp;&amp; 'Transactions'[CATEGORY] &lt;&gt; "Exports"
                 &amp;&amp; 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS"
             ),
@@ -6136,62 +5484,9 @@
                 ALL('Transactions'),
                 'Transactions'[TRANS_DATE] &gt;= DATE(vMaxYear, vMaxMonth, 1)
                 &amp;&amp; 'Transactions'[WEEK] = vMaxWeek
-                &amp;&amp; 'Transactions'[WEEKDAY] = "Tue"
+                &amp;&amp; 'Transactions'[WEEKDAY] = "Wed"
                 &amp;&amp; 'Transactions'[CATEGORY] &lt;&gt; "Exports"
                 &amp;&amp; 'Transactions'[ITEM_PACKSIZE</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B59" s="2" t="inlineStr">
-        <is>
-          <t>My new sheet (2)</t>
-        </is>
-      </c>
-      <c r="C59" s="2" t="inlineStr">
-        <is>
-          <t>qsSimpleKPI</t>
-        </is>
-      </c>
-      <c r="D59" s="2" t="inlineStr">
-        <is>
-          <t>Measure</t>
-        </is>
-      </c>
-      <c r="E59" s="2" t="inlineStr">
-        <is>
-          <t>['=\r\n(sum({&lt;TRANS_DATE={"&lt;$(vPrevDate)"}, WEEK={$(vMaxWeek)}, WEEKDAY = {\'Wed\'}, CATEGORY-={\'Exports\'}, ITEM_PACKSIZE_GROUP={\'BALERS\'}&gt;}MonthWeight)\n+ sum({&lt;TRANS_DATE={"&gt;=$(vPrevDate)"}, WEEK={$(vMaxWeek)}, WEEKDAY = {\'Wed\'}, CATEGORY-={\'Exports\'}, ITEM_PACKSIZE_GROUP={\'BALERS\'}&gt;}Weight))/\n(\n((sum({&lt;MONTHNO={$(vMaxMonth)}, CATEGORY-={\'Exports\'}, ITEM_PACKSIZE_GROUP={\'BALERS\'}&gt;} AOPVol)/\nNetWorkDays(monthstart(Makedate(vMaxYear,vMaxMonth)),MonthEnd(Makedate(vMaxYear,vMaxMonth)),$(vWorkingDays))))\n)']</t>
-        </is>
-      </c>
-      <c r="F59" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-DIVIDE(
-    ADD(
-        SUMX(
-            FILTER(
-                ALL('Transactions'),
-                'Transactions'[TRANS_DATE] &lt; DATE(vMaxYear, vMaxMonth, 1)
-                &amp;&amp; 'Transactions'[WEEK] = vMaxWeek
-                &amp;&amp; 'Transactions'[WEEKDAY] = "Wed"
-                &amp;&amp; 'Transactions'[CATEGORY-] &lt;&gt; "Exports"
-                &amp;&amp; 'Transactions'[ITEM_PACKSIZE_GROUP] = "BALERS"
-            ),
-            'Transactions'[MonthWeight]
-        ),
-        SUMX(
-            FILTER(
-                ALL('Transactions'),
-                'Transactions'[TRANS_DATE] &gt;= DATE(vMaxYear, vMaxMonth, 1)
-                &amp;&amp; 'Transactions'[WEEK] = vMaxWeek
-                &amp;&amp; 'Transactions'[WEEKDAY] = "Wed"
-                &amp;&amp; 'Transactions'[CATEGORY-] &lt;&gt; "Exports"
-                &amp;&amp; 'Transactions'[ITEM_P</t>
         </is>
       </c>
     </row>
@@ -6363,7 +5658,7 @@
       <c r="F63" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-FORMAT(DIVIDE(DIVIDE(SUMX(FILTER(ALL('Date'), 'Date'[MonthNo] = MAX('Date'[MonthNo])), [AOPVol]), NETWORKDAYS.INTL(STARTOFMONTH('Date'[Date]), ENDOFMONTH('Date'[Date]), $(vWorkingDays)) * NETWORKDAYS.INTL(STARTOFMONTH('Date'[Date]), TODAY(), $(vWorkingDays))), 1000), "#,##0")</t>
+FORMAT(DIVIDE(DIVIDE(SUMX(FILTER(ALL('Date'), 'Date'[MonthNo] = MAX('Date'[MonthNo])), [AOPVol]), DATEDIFF(EOMONTH(MAX('Date'[Date]), 0), EOMONTH(MAX('Date'[Date]), -1), WEEKDAY)), 1000), "#,##0")</t>
         </is>
       </c>
     </row>
@@ -6398,32 +5693,35 @@
           <t xml:space="preserve">
 SUMX(
     FILTER(
-        ALLSELECTED(TableName[Dimension]),
-        TableName[Dimension] = "Month"
-    ),
-    TableName[LastEstimate]
-)/
-DIVIDE(
-    SUMX(
-        FILTER(
-            ALLSELECTED(TableName[MONTHNO]),
-            TableName[MONTHNO] = $(vMaxMonth)
-        ),
-        TableName[AOPVol]
+        ALLSELECTED(TableName),
+        MONTHNO = vMaxMonth
     ),
     DIVIDE(
-        NETWORKDAYS.INTL(
-            STARTOFMONTH(MAKEDATE(vMaxYear, vMaxMonth)),
-            ENDOFMONTH(MAKEDATE(vMaxYear, vMaxMonth)),
-            $(vWorkingDays)
+        SUM(
+            FILTER(
+                TableName,
+                MONTHNO = vMaxMonth &amp;&amp; TRANS_DATE &lt; vPrevDate
+            ),
+            MonthWeight
+        ) +
+        SUM(
+            FILTER(
+                TableName,
+                MONTHNO = vMaxMonth &amp;&amp; TRANS_DATE &gt;= vPrevDate
+            ),
+            Weight
         ),
-        NETWORKDAYS.INTL(
-            STARTOFMONTH(MAKEDATE(vMaxYear, vMaxMonth)),
-            MAKEDATE(vMaxYear, vMaxMonth, DAY(TODAY())),
-            $(vWorkingDays)
-        )
-    )
-)</t>
+        DIVIDE(
+            SUM(TableName[AOPVol]),
+            MULTIPLY(
+                NETWORKDAYS.INTL(
+                    STARTOFMONTH(MAKEDATE(vMaxYear, vMaxMonth, 1)),
+                    ENDOFMONTH(MAKEDATE(vMaxYear, vMaxMonth, 1)),
+                    vWorkingDays
+                ),
+                NETWORKDAYS.INTL(
+                    STARTOFMONTH(MAKEDATE(vMaxYear, vMaxMonth, 1)),
+                    MAKEDATE(vMaxYear, v</t>
         </is>
       </c>
     </row>
@@ -6664,7 +5962,7 @@
       <c r="F70" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-FORMAT(SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &lt;= $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek)), [MonthWeight]) + SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &gt;= $(vPrevDate) &amp;&amp; 'Table'[WEEK] = $(vMaxWeek)), [Weight])/1000, "# ##0")</t>
+FORMAT(SUMX(FILTER(ALL('Table'), 'Table'[TRANS_DATE] &lt;= $(vMaxDate)), 'Table'[Weight])/1000, "# ##0")</t>
         </is>
       </c>
     </row>
@@ -6790,8 +6088,8 @@
     CALCULATE (
         SUM ( 'CWO_Status'[CWO - QTY_ORDER] ),
         FILTER (
-            ALL ( 'Calendar' ),
-            'Calendar'[Week] = WEEKNUM ( TODAY () )
+            ALL ( 'WEEK' ),
+            'WEEK'[WEEK] = WEEK ( TODAY () )
         )
     )
 )</t>
@@ -6933,7 +6231,7 @@
       <c r="F77" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-DIVIDE(VALUE(3), SUMX(FILTER(ALLSELECTED('CWO'), 'CWO'[WEEK] = FORMAT(TODAY(), "WW"), 'CWO'[CWO_Status] = "Active"), 'CWO'[CWO - QTY_ORDER]))</t>
+DIVIDE(VALUE(3), SUMX(FILTER(ALLSELECTED('CWO'), 'CWO'[WEEK] = WEEK(TODAY()), 'CWO'[CWO_Status] = "Active"), 'CWO'[CWO - QTY_ORDER]))</t>
         </is>
       </c>
     </row>
@@ -7794,7 +7092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7803,8 +7101,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31.2" customWidth="1" min="1" max="1"/>
-    <col width="19.2" customWidth="1" min="2" max="2"/>
-    <col width="9742.799999999999" customWidth="1" min="3" max="3"/>
+    <col width="14.4" customWidth="1" min="2" max="2"/>
+    <col width="16.8" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7832,1545 +7130,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>SAPRoute:</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD distinct replace(replace(subfield([Customer - Customer Level 01 (Key)],'.',2),'[',''),']','') as KAM, 
-     replace(replace(subfield([Route - Route Level 01 (Key)],'.',2),'[',''),']','') as OriginalSAPRoute
-FROM
-[lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\ESDOV0001-ZE_ESDOV0001_C000_00001.QVD]
-(qvd);
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>SAPRouteNo</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD distinct SLSMAN_CD as SAPRoute, 
-     USER_DEFINE3 As OriginalSAPRoute,
-     USER_DEFINE2 As SAPDTSRegion,
-     BU_CD
-FROM
-[lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\MST_SLSMAN.qvd]
-(qvd);
-left join (SAPRoute)
-load * resident SAPRouteNo;
-drop table SAPRouteNo;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>NewDTSRegions</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD
-    REF_PARAM as BU_CD,
-    REF_VALUE as SAP_ROUTE_LOCATION
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\SET_REF.qvd]
-(qvd);
-left join (SAPRoute)
-load * resident NewDTSRegions;
-drop table NewDTSRegions;
-left join (RouteCustomerDetails)
-load * resident SAPRoute;
-drop table SAPRoute;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>RC</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct CUST_ID,
-//KAM,
-SAP_ROUTE_LOCATION,
-MAJOR_GROUP
-//DTS_REGION,
-//SAPDTSRegion
-resident RouteCustomerDetails;
-left join (OpenOrders)
-load *
-resident RC;
-drop table RC;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Tmp</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load *,
-num(date(floor(if(upper(left(SAP_ROUTE_LOCATION,6))='ISANDO' or upper(left(SAP_ROUTE_LOCATION,5))='PAROW',if(wildmatch(WeekDay([Date(CREATE_DT)]),'Thu','Fri'),[Date(CREATE_DT)]+4,[Date(CREATE_DT)]+2),if(wildmatch(WeekDay([Date(CREATE_DT)]),'Thu','Fri'),[Date(CREATE_DT)]+4,[Date(CREATE_DT)]+2))),'YYYY/MM/DD')) as TDate,
-num(date(floor([Date(CREATE_DT)]),'YYYY/MM/DD')) as OpenOrderDate,
-num(date(floor(if(upper(left(SAP_ROUTE_LOCATION,6))='ISANDO' or upper(left(SAP_ROUTE_LOCATION,5))='PAROW',if(wildmatch(WeekDay([Date(CREATE_DT)]),'Thu','Fri'),[Date(CREATE_DT)]+4,[Date(CREATE_DT)]+2),if(wildmatch(WeekDay([Date(CREATE_DT)]),'Thu','Fri'),[Date(CREATE_DT)]+4,[Date(CREATE_DT)]+2))),'YYYY/MM/DD')) as OpenOrderDeliveryDate,
-CUST_ID&amp;'-'&amp;ITEM_ID&amp;'-'&amp;num(date(floor(if(upper(left(SAP_ROUTE_LOCATION,6))='ISANDO' or upper(left(SAP_ROUTE_LOCATION,5))='PAROW',if(wildmatch(WeekDay([Date(CREATE_DT)]),'Thu','Fri'),[Date(CREATE_DT)]+4,[Date(CREATE_DT)]+2),if(wildmatch(WeekDay([Date(CREATE_DT)]),'Thu','Fri'),[Date(CREATE_DT)]+4,[Date(CREATE_DT)]+2))),'YYYY/MM/DD'))&amp;'-'&amp;ORDER_NO as OpenOrderLink
-resident OpenOrders
-where MAJOR_GROUP&lt;&gt;'EXPORTS';
-rename field ORDER_STATUS to OpenOrderStatus;
-drop table OpenOrders;
-rename table Tmp to OpenOrders;
-drop field SAP_ROUTE_LOCATION,MAJOR_GROUP from OpenOrders;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>RC2</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct CUST_ID,
-//KAM,
-//SAP_ROUTE_LOCATION,
-MAJOR_GROUP
-//DTS_REGION,
-//SAPDTSRegion
-resident RouteCustomerDetails;
-///$tab Section 2
-drop table ItemDetail;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>ItemDetail</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD distinct 
-	AutoNumber("NP Number") AS ITEM_DETAILS,
-    maxstring(upper("NP Description Short")) as ITEM_NAME, 
-	maxstring(upper("NP Brand Group")) as ITEM_BRAND_GROUP, 
- 	maxstring(upper("NP Brand")) as ITEM_BRAND, 
-    "NP Number" as ITEM_ID,
-    maxstring("SAP Number") as SAP_ITEM_ID,
-    maxstring("NP Flavour") as ITEM_FLAVOUR,
-    maxstring("NP Flavour ID") as ITEM_FLAVOUR_ID,
-    maxstring(upper("Core/Value")) as [CORE/VALUE CO],
-    maxstring(upper("NP Packsize")) as ITEM_PACKSIZE,
-    maxstring(upper(if(trim(upper("NP PacksizeGroup"))='XL','EXTRA LARG',"NP PacksizeGroup"))) as ITEM_PACKSIZE_GROUP
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\vQlikSense_Product.qvd]
-(qvd)
-group by "NP Number";
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>Itm2</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD AutoNumber(ItemID) as ITEM_DETAILS,
-    ItemID as SAP_ITEM_ID,
-    maxstring(upper("SKU Description")) as ITEM_NAME,
-    maxstring(upper("Item Brand")) as ITEM_BRAND,
-    maxstring(upper(if(wildmatch(upper("Item Brand"),'DORITOS','DORITOS 3D BUGLES','DORITOS JACKED'),'TORTILLA CHIPS',"Item Brand Group"))) as ITEM_BRAND_GROUP,
-    maxstring(upper("Item Packsize Group")) as ITEM_PACKSIZE_GROUP,
-    maxstring(upper("Item Packsize")) as ITEM_PACKSIZE,
-    maxstring(upper("Core/ValueCo")) as [CORE/VALUE CO],
-    ItemID  as ITEM_ID
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/Excel/SalesModel/AOP/AOP 2021.xlsx]
-(ooxml, embedded labels, table is [New Item Link])
-group by ItemID;
-concatenate(ItemDetail)
-load * resident Itm2;
-drop table Itm2;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Tmp2</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD maxstring(ITEM_DETAILS) as ITEM_DETAILS,
-    maxstring(ITEM_NAME) as ITEM_NAME, 
-	maxstring(ITEM_BRAND_GROUP) as ITEM_BRAND_GROUP, 
- 	maxstring(ITEM_BRAND) as ITEM_BRAND, 
-    ITEM_ID,
-    maxstring(SAP_ITEM_ID) as SAP_ITEM_ID,
-    maxstring(ITEM_FLAVOUR) as ITEM_FLAVOUR,
-    maxstring(ITEM_FLAVOUR_ID) as ITEM_FLAVOUR_ID,
-    maxstring([CORE/VALUE CO]) as [CORE/VALUE CO],
-    maxstring(ITEM_PACKSIZE) as ITEM_PACKSIZE,
-    maxstring(ITEM_PACKSIZE_GROUP) as ITEM_PACKSIZE_GROUP
-resident ItemDetail
-group by ITEM_ID;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>Tmp</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD ITEM_DETAILS,
-    ITEM_NAME, 
-	if(len(ITEM_BRAND_GROUP)=0,'OTHER',ITEM_BRAND_GROUP) as ITEM_BRAND_GROUP, 
- 	if(len(ITEM_BRAND)=0,'OTHER',ITEM_BRAND) as ITEM_BRAND, 
-    ITEM_ID,
-    SAP_ITEM_ID as SAP_ITEM_ID,
-    if(len(ITEM_FLAVOUR)=0,'OTHER',ITEM_FLAVOUR) as ITEM_FLAVOUR,
-    if(len(ITEM_FLAVOUR_ID)=0,'OTHER',ITEM_FLAVOUR_ID) as ITEM_FLAVOUR_ID,
-    if(len([CORE/VALUE CO])=0,'OTHER',[CORE/VALUE CO]) as [CORE/VALUE CO],
-    if(len(ITEM_PACKSIZE)=0 or isnull(ITEM_PACKSIZE),'OTHER',ITEM_PACKSIZE) as ITEM_PACKSIZE,
-    if(len(ITEM_PACKSIZE_GROUP)=0,'OTHER',ITEM_PACKSIZE_GROUP) as ITEM_PACKSIZE_GROUP
-resident Tmp2;
-drop table ItemDetail;
-drop table Tmp2;
-rename table Tmp to ItemDetail;
-///$tab Sales
-LIB CONNECT TO '196.6.3.40 (NewsPage) (cwwpvt_zaqlickviewadmin)';
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>QVUpdateTmp</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOAD "TTRANS_ID",
-    COMPANY,
-    "BRN_ID",
-    BRANCH,
-    "ROU_LOC_ID",
-    "ROUTE_LOCATION",
-    "ROU_ID",
-    ROUTE,
-    "ROU_CAT_ID",
-    KAM,
-    "CUST_ID",
-    "CUSTOMER_NAME",
-    "CUSTOMER_NAME2",
-    DMDGROUP,
-    BLOCK,
-    STATUS,
-    "CLASS_ID",
-    "EXPENSE_ID",
-    "KEY_ACCOUNT",
-    "KEY_ACCOUNT_CUST_ID",
-    CATEGORY,
-    "MAJOR_GROUP",
-    "GROUP",
-    "GROUP_CUST_ID",
-    REGION,
-    "REGION_CUST_ID",
-    "SUB_REGION",
-    SEGMENT,
-    "SUB_SEGMENT",
-    "DTS_REGION_GROUP",
-    "DTS_REGION",
-    "YEAR",
-    PERIOD,
-    "MONTH",
-    "WEEK",
-    "ACTUAL_DATE",
-    "DES_ID",
-    "ITEM_ID",
-    "ITEM_NAME",
-    "ITEM_BRAND_GROUP",
-    "ITEM_BRAND",
-    "ITEM_PACKSIZE_GROUP",
-    "ITEM_PACKSIZE",
-    "PRODUCT_TYPE",
-    "JDA_PRD",
-    "TYPE",
-    REASON,
-    CasePrice,
-    Cases,
-    Gross,
-    Discount,
-    Nett,
-    "INVOICE_NUMBER",
-    "TRANS_DATE",
-    Weight,
-    Units,
-    "PO_NO",
-    "inv_no_ref",
-    "GRN_NO",
-    "CLAIM_NO",
-    "Shiped_to_GLN",
-    "FULL_IND",
-    "CUST_TYPE";
-SQL SELECT "TTRANS_ID",
-    COMPANY,
-    "BRN_ID",
-    BRANCH,
-    "ROU_LOC_ID",
-    "ROUTE_LOCATION",
-    "ROU_ID",
-    ROUTE,
-    "ROU_CAT_ID",
-    KAM,
-    "CUST_ID",
-    "CUSTOMER_NAME",
-    "CUSTOMER_NAME2",
-    DMDGROUP,
-    BLOCK,
-    STATUS,
-    "CLASS_ID",
-    "EXPENSE_ID",
-    "KEY_ACCOUNT",
-    "KEY_ACCOUNT_CUST_ID",
-    CATEGORY,
-    "MAJOR_GROUP",
-    "GROUP",
-    "GROUP_CUST_ID",
-    REGION,
-    "REGION_CUST_ID",
-    "SUB_REGION",
-    SEGMENT,
-    "SUB_SEGMENT",
-    "DTS_REGION_GROUP",
-    "DTS_REGION",
-    "YEAR",
-    PERIOD,
-    "MONTH",
-    "WEEK",
-    "ACTUAL_DATE",
-    "DES_ID",
-    "ITEM_ID",
-    "ITEM_NAME",
-    "ITEM_BRAND_GROUP",
-    "ITEM_BRAND",
-    "ITEM_PACKSIZE_GROUP",
-    "ITEM_PACKSIZE",
-    "PRODUCT_TYPE",
-    "JDA_PRD",
-    "TYPE",
-    REASON,
-    CasePrice,
-    Cases,
-    Gross,
-    Discount,
-    Nett,
-    "INVOICE_NUMBER",
-    "TRANS_DATE",
-    Weight,
-    Units,
-    "PO_NO",
-    "inv_no_ref",
-    "GRN_NO",
-    "CLAIM_NO",
-    "Shiped_to_GLN",
-    "FULL_IND",
-    "CUST_TYPE"
-FROM "SIMBA_DMS_LIVE".dbo."vQlikSense_Update_TodaySales";
-NoConcatenate
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>QlikViewUpdate</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOAD 
-//	AutoNumber(DES_ID &amp; '-' &amp; COMPANY &amp; '-' &amp; BRN_ID &amp; '-' &amp; BRANCH &amp; '-' &amp; ROU_LOC_ID &amp; '-' &amp; ROUTE_LOCATION &amp; '-' &amp; ROU_ID &amp; '-' &amp; ROUTE &amp; '-' &amp; KAM &amp; '-' &amp; CUST_ID &amp; '-' &amp; 
-//	CUSTOMER_NAME &amp; '-' &amp; KEY_ACCOUNT &amp; '-' &amp; KEY_ACCOUNT_CUST_ID &amp; '-' &amp; CATEGORY &amp; '-' &amp; MAJOR_GROUP &amp; '-' &amp; [GROUP] &amp; '-' &amp; GROUP_CUST_ID &amp; '-' &amp; 
-//	REGION &amp; '-' &amp; REGION_CUST_ID &amp; '-' &amp; SUB_REGION &amp; '-' &amp; SEGMENT &amp; '-' &amp; SUB_SEGMENT &amp; '-' &amp; DTS_REGION_GROUP &amp; '-' &amp; DTS_REGION) AS ALL_DETAILS,
-//	AutoNumber(ITEM_ID &amp; '-' &amp; ITEM_NAME &amp; '-' &amp; ITEM_BRAND_GROUP &amp; '-' &amp; ITEM_BRAND &amp; '-' &amp;ITEM_PACKSIZE_GROUP &amp; '-' &amp; ITEM_PACKSIZE) AS ITEM_DETAILS,
-//	AutoNumber(ITEM_ID) AS ITEM_DETAILS,
-//	AutoNumber(LTRIM(RTRIM(REGION)) &amp; '-' &amp; LTRIM(RTRIM(MAJOR_GROUP)) &amp; '-' &amp; LTRIM(RTRIM([GROUP])) &amp; '-' &amp; LTRIM(RTRIM(CATEGORY)) &amp; '-' &amp; LTRIM(RTRIM(SEGMENT)) &amp; '-' &amp; 
-//	LTRIM(RTRIM(ITEM_BRAND)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_PACKSIZE_GROUP)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_PACKSIZE)) &amp; '-' &amp; LTRIM(RTRIM(WEEK))) AS BOSSLink,
-//	AutoNumber(LTRIM(RTRIM(ITEM_BRAND)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_PACKSIZE_GROUP)) &amp; '-' &amp; LTRIM(RTRIM(NewMonth)) &amp; '-' &amp; LTRIM(RTRIM(YEAR))) AS ForecastKey,
-//	AutoNumber(LTRIM(RTRIM(ITEM_ID)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_NAME)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_BRAND_GROUP)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_BRAND)) &amp; '-' &amp; 
-//     LTRIM(RTRIM(ITEM_PACKSIZE_GROUP)) &amp; '-' &amp; LTRIM(RTRIM(ITEM_PACKSIZE))) AS NewProductKey,
-//	ITEM_BRAND &amp; ' - '&amp;ITEM_PACKSIZE_GROUP &amp; '_' &amp; YEAR &amp; '_' &amp; MONTH as ForecastLink,
-//    AutoNumber(INVOICE_NUMBER&amp;'-'&amp;ITEM_ID&amp;'-'&amp;CUST_ID&amp;'-'&amp;EXPENSE_ID) as SalesLink,
-	RowNo() AS RowNumber,
-    ITEM_ID,
-    CUST_ID,
-    ITEM_ID as ITEM_ID1,
-	CUST_ID as LINKCUST_ID,
-	CUST_ID as CUST_ID1,
-	CLASS_ID,
-	EXPENSE_ID,
-	//*****
-//	ITEM_PACKSIZE_GROUP,
-//  ITEM_PACKSIZE,
-    //*****
-////	TTRANS_ID, 
-//	INDICATOR, 
-	YEAR AS qvYEAR, 
-	PERIOD AS qvPERIOD, 
-	MONTH AS qvMONTH, 
-	WEEK AS qvWEEK, 
-//	ACTUAL_DATE, 
-	Capitalize(TYPE) as TYPE, 
-	REASON, 
-	CasePrice, 
-	Gross as GrossBossView, 
-     IF(Capitalize(TYPE)='Buyback',fabs(Gross)*-1,0) AS GrossBuyback,
-     IF(Capitalize(TYPE)='Return',fabs(Gross)*-1,0) AS GrossReturn,
-     IF(Capitalize(TYPE)='Export Credit',fabs(Gross)*-1,0) AS GrossExpcred,
-     IF(Capitalize(TYPE)&lt;&gt;'Return' OR Capitalize(TYPE)&lt;&gt;'Buyback',fabs(Gross),0) AS GrossEx,
-	Discount, 
-	Nett AS Invoice, 
-	IF(Cases &lt;&gt; 0 OR Units &lt;&gt; 0,CasePrice / (Units / Cases),0) AS UnitPrice,
-	INVOICE_NUMBER, 
-	if(Capitalize(TYPE)='Buyback' or Capitalize(TYPE)='Return',Cases*-1,Cases) as Cases,
-	if(Capitalize(TYPE)='Buyback' or Capitalize(TYPE)='Return',Units*-1,Units) as Units,
-	if(Capitalize(TYPE)='Buyback' or Capitalize(TYPE)='Return',Weight*-1,Weight) as Weight,	 
-//	Capitalize([Data Source]) as [Data Source], 
-	date(floor(TRANS_DATE),'YYYY/MM/DD') as TRANS_DATE2,
-//	text(date(TRANS_DATE,'YYYY/MM/DD')) as TRANS_DATE_LINK,
-//	DateTime,
-//	//*****
-	//Time(DateTime) as TRANS_TIME,
-//	left(subfield(DateTime,' ' ,2),5) as Transaction_Time,
-	//*****      
-	date(floor(TRANS_DATE),'DD/MM') as TRANS_DM,      
-	Num(Month(floor(TRANS_DATE)),'00') &amp; '/' &amp; Num(Day(floor([TRANS_DATE])),'00') as TRANS_DM2, 
-//	YearMonth, 
-//	NewMonth, 
-//	QUARTER AS qvQUARTER, 
-//	SIMBAQUARTER, 
-//	SimbaYearPeriod,
-    [DMDGROUP],
-      [JDA_PRD],
-      [CUST_TYPE],
-      inv_no_ref,
-     FULL_IND,
-     CUST_ID&amp;'-'&amp;ITEM_ID&amp;'-'&amp;num(floor(TRANS_DATE))&amp;'-'&amp;INVOICE_NUMBER as SalesLink
-Resident 
-	QVUpdateTmp
-where not WildMatch(CUST_ID,419524,428140);
-; //where YEAR = '2013';
-Drop Table QVUpdateTmp;
-//------------------------------------------------------------------------------------------------
-LEFT JOIN (QlikViewUpdate)
-LOAD
-	RowNumber,
-	(GrossEx + GrossBuyback + GrossReturn) AS Gross,
-//	(GrossEx + GrossBuyback + GrossBuyback + GrossReturn + GrossExpcred) AS GrossFin
-IF(Capitalize(TYPE)='Buyback',GrossBuyback,
-     IF(Capitalize(TYPE)='Return',0,
-     IF(Capitalize(TYPE)='Export Credit',GrossExpcred,
-     GrossEx))) as GrossFin,
-     If(Discount&gt;0 or Discount&lt;0,1,0) as DiscountInd,
-     num(TRANS_DATE2) as TRANS_DATE
-RESIDENT 
-	QlikViewUpdate;
-//------------------------------------------------------------------------------------------------
-left join (QlikViewUpdate)
-load * resident RC2;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>Tmp</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load * resident QlikViewUpdate
-where "MAJOR_GROUP"&lt;&gt;'EXPORTS';
-drop table QlikViewUpdate;
-rename table Tmp to QlikViewUpdate;
-drop field "MAJOR_GROUP" from QlikViewUpdate;
-// Tmp:
-// NoConcatenate
-// load CUST_ID&amp;'-'&amp;ITEM_ID&amp;'-'&amp;num(floor(TRANS_DATE))&amp;'-'&amp;INVOICE_NUMBER as SalesLink,
-// CUST_ID,
-// ITEM_ID,
-// TRANS_DATE,
-// INVOICE_NUMBER,
-// sum(GrossFin) as GrossFin,
-// sum(Weight) as Weight
-// resident QlikViewUpdate
-// group by CUST_ID,
-// ITEM_ID,
-// TRANS_DATE,
-// INVOICE_NUMBER;
-// drop table QlikViewUpdate;
-// rename table Tmp to QlikViewUpdate;
-//LIB CONNECT TO '196.6.3.46 - NewspageQA (cwwpvt_zaqlickviewadmin)';
-///$tab Monthly Sales
-let vTDate=Today()-1;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>MonthlySales</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD
-    CUST_ID,
-    ITEM_ID,
-    TRANS_DATE,
-    TYPE as MonthTYPE,
-    GrossFin as MonthGrossFin,
-    GrossReturn as MonthGrossReturn,
-    Invoice as MonthInvoice,
-    Weight as MonthWeight,
-    AOPVal,
-    AOPVol,
-    AOPInvoiceVal,
-    CUST_ID&amp;'-'&amp;ITEM_ID&amp;'-'&amp;TRANS_DATE as MonthlyLink
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\DailyDashboard\MonthAndWeekSalesAndAOPLast2Months.qvd]
-(qvd)
-where not WildMatch(CUST_ID,419524,428140);
-left join (MonthlySales)
-load * resident RC2;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>Tmp</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load * resident MonthlySales
-where MAJOR_GROUP&lt;&gt;'EXPORTS';
-drop table MonthlySales;
-rename table Tmp to MonthlySales;
-drop field MAJOR_GROUP from MonthlySales;
-///$tab Orders To Be Delivered
-// OTBD:
-// LIB CONNECT TO '196.6.3.40 (NewsPage) (cwwpvt_zaqlickviewadmin)';
-// LOAD num("DELIVERY_DAY") as TRANS_DATE,
-//     "CUST_CD" as CUST_ID,
-//     "ORDER_NO" as ORDER_NUMBER,
-//     "ORDER_STATUS" as OrderToBeDelStatus,
-// //    "CREATE_DT" as ORDER_DATE,
-//     "PRD_CD" as ITEM_ID,
-//     "PRD_QTY" as ORDERED_QTY,
-//     KGs as ORDERED_KG,
-//     "GROSS_AMT" as ORDERED_AMOUNT;
-// SQL SELECT "DELIVERY_DAY",
-//     "CUST_CD",
-//     "ORDER_NO",
-//     "ORDER_STATUS",
-//     "CREATE_DT",
-//     "PRD_CD",
-//      "PRD_QTY",
-//     KGs,
-//     "GROSS_AMT"
-// FROM "SIMBA_DMS_LIVE".dbo."vQliksense_OrdersToBeDelivered";
-// OrdersToDeliver:
-// load TRANS_DATE,
-// CUST_ID,
-// ORDER_NUMBER,
-// ITEM_ID,
-// OrderToBeDelStatus,
-// TRANS_DATE&amp;'-'&amp;CUST_ID&amp;'-'&amp;ITEM_ID&amp;'-'&amp;ORDER_NUMBER&amp;'-'&amp;OrderToBeDelStatus as OrdersToDeliverLink,
-// sum(ORDERED_QTY) as ORDERED_QTY,
-// sum(ORDERED_KG) as ORDERED_KG,
-// sum(ORDERED_AMOUNT) as ORDERED_AMOUNT
-// resident OTBD
-// where not WildMatch(CUST_ID,419524,428140)
-// group by TRANS_DATE,
-// CUST_ID,
-// ITEM_ID,
-// OrderToBeDelStatus,
-// ORDER_NUMBER;
-// drop table OTBD;
-///$tab Last Estimate
-// LEMonthAndWeek:
-// LOAD
-//     "Dimension",
-//     DimensionValue,
-//     "Measure" as LastEstimate
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/Excel\SalesModel\LE.xlsx]
-// (ooxml, embedded labels, table is LE)
-// where "Dimension"&lt;&gt;'DTS REGION';
-// LEMonthAndWeek:
-// LOAD DimensionValue as DTS_REGION,
-//     "Measure" as LastDTSEstimate
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/Excel\SalesModel\LE.xlsx]
-// (ooxml, embedded labels, table is LE)
-// where "Dimension"='DTS REGION';
-///$tab JDA
-// JDATmp:
-// CrossTable(Date, JDACases, 3)
-// LOAD [DC MAP], 
-//      [ITEM NUMBER] as ITEM_ID, 
-//      [ITEM NAME], 
-//      *
-// FROM
-// [\\11.69.64.36\d$\QS\QSData\Excel\Daily Sales Report\JDA DC *.xlsx]
-// (ooxml, embedded labels, table is Sheet2); 
-// JDAtmp2:
-// NoConcatenate
-// load [DC MAP],
-// ITEM_ID,
-// num(num#(Date)) as TRANS_DATE,
-// JDACases,
-// Date&amp;'-'&amp;ITEM_ID&amp;'-'&amp;[DC MAP] as JDALink
-// resident JDATmp
-// where isnum(Date)=0;
-// drop table JDATmp;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>JDAtmp2</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD
-    "DC MAP",
-    ITEM_ID,
-    TRANS_DATE,
-    JDACases,
-    TRANS_DATE&amp;'-'&amp;ITEM_ID&amp;'-'&amp;[DC MAP] as JDALink
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/Excel/Daily Sales Report/JDASplit.qvd]
-(qvd); 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>Conversion</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD distinct
-    num(PRD_CD) as ITEM_ID,
-//    CONV_FACTOR as CFactor,
-//    GROSS_WEIGHT as ConWeight,
-//    WEIGHT_UNIT as ConUnit,
-    (if(WEIGHT_UNIT='kg',GROSS_WEIGHT,(GROSS_WEIGHT* 0.001)))*CONV_FACTOR as ConFac
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\MST_PRDUOM.qvd]
-(qvd)
-where     UOM_CD='CS';
-left join (JDAtmp2)
-load * resident Conversion;
-drop table Conversion;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>JDA</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">load *,
-(JDACases*ConFac) as JDAValue
-resident JDAtmp2;
-drop table JDAtmp2;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>JDALink</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-Load distinct [DC MAP], 
-ITEM_ID,
-TRANS_DATE,
-JDALink
-resident JDA;
-drop fields [DC MAP], ITEM_ID, TRANS_DATE from JDA;
-///$tab CWO
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>CWO</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOAD
-    [CWO - QTY_INVOICED],
-    [CWO - QTY_ORDER],
-    num("Date") as TRANS_DATE,
-    "Dimension - Product Code" as ITEM_ID,
-    CUST_ID,
-    %CWO_ACT_INACT_LINK,
-    num("Date")&amp;'-'&amp;"Dimension - Product Code" &amp;'-'&amp;CUST_ID as CWOLink
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD/Consolidated - Sales View/Operations.qvd]
-(qvd)
-where not WildMatch(CUST_ID,419524,428140) and YEAR("Date")=$(vYear) and num(month("Date"))=$(vMonthnum); 
-left join (CWO)
-load * resident RC2;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Tmp</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load * resident CWO
-where MAJOR_GROUP&lt;&gt;'EXPORTS';
-drop table CWO;
-rename table Tmp to CWO;
-drop field MAJOR_GROUP from CWO;
-drop table RC2;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>LinkTableCWO</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct TRANS_DATE,
-CUST_ID,
-ITEM_ID,
-CWOLink
-resident CWO;
-drop fields TRANS_DATE,
-CUST_ID,
-ITEM_ID from CWO;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>CWO_STATUS</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD distinct
-    CWO_Status,
-    %CWO_ACT_INACT_LINK
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD/Consolidated - Sales View/CWO_Status.qvd]
-(qvd);
-///$tab CDC Key
-// Data2:
-// LOAD
-//     DDATE as DDATE,
-//     Num(date#(left(RPROUTE,8),'YYYYMMDD')) as NumDateP,
-//     num(Date#(DDATE, 'DD-MMM-YYYY')) as NumDate,
-//     right(RPROUTE,6) as ROUTEID,
-//     STATUS,
-//     ORDER_ID,
-//     "Customer ID" as CUST_ID,
-// //    SHIP_DOCK,
-// //    RPROUTE,
-//     SKU_ID as ITEM_ID,
-//     QTYORDERED,
-// //    QTYTASKED,
-// //    QTYPICKED,
-// //    PALLETSPICKED,
-// //    PALLETSOUT,
-// //    FULFILLED,
-// //    RATIO_1_TO_2,
-// //    Plant,
-//     CustomerName as CustomerNameVR
-// //    if(Left(ORDER_ID,2) = 'SO','SO', if(Left(ORDER_ID,2) = 'VQ','VQ',if(Left(ORDER_ID,2) = 'IF','IF'))) as Bucket,
-// //      if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &lt;= 2 ,'0-2 Days', 
-// //    if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &gt;2 and today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &lt;= 5 ,'3-5 Days',
-//     //if(today() - CREATE_DT &gt;5 and today() - CREATE_DT &lt;= 10 ,'6-10 Days',
-// //    if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &gt; 5 ,'Greater than 5 Days'))) as AgeBucket
-//     //'Primary' as Primary,
-//    // 'Van Request' As VanRequest
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\CDCKeyAccount\IsandoOrderMan.qvd]
-// (qvd);
-// MyDays:
-// NoConcatenate
-// load distinct NumDate as DDate2
-// resident Data2
-// where wildmatch(STATUS,'Released','Allocated','In Progress','Picked');
-// Data:
-// NoConcatenate
-// load * resident Data2
-// where exists(DDate2, NumDate);
-// drop table Data2;
-// drop table MyDays;
-// //exit script;
-// Data2:
-// NoConcatenate
-// LOAD
-//     DDATE as DDATE,
-// //    date(date#(left(RPROUTE,8),'YYYYMMDD'),'YYYY/MM/DD') as DDATE,
-//     Num(date#(left(RPROUTE,8),'YYYYMMDD')) as NumDateP,
-//     num(Date#(DDATE, 'DD-MMM-YYYY')) as NumDate,
-//     right(RPROUTE,6) as ROUTEID,
-//     STATUS,
-//     upper(ORDER_ID) as ORDER_ID,
-//     "Customer ID" as CUST_ID,
-// //    SHIP_DOCK,
-//     SKU_ID as ITEM_ID,
-//     QTYORDERED,
-// //     RPROUTE,
-// //     QTYTASKED,
-// //     QTYPICKED,
-// //     PALLETSPICKED,
-// //     PALLETSOUT,
-// //     FULFILLED,
-// //     RATIO_1_TO_2,
-// //     Plant,
-//      CustomerName as CustomerNameVR
-// //     if(Left(ORDER_ID,2) = 'SO','SO', if(Left(ORDER_ID,2) = 'VQ','VQ',if(Left(ORDER_ID,2) = 'IF','IF'))) as Bucket,
-// //       if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &lt;= 2 ,'0-2 Days', 
-// //     if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &gt;2 and today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &lt;= 5 ,'3-5 Days',
-// //     //if(today() - CREATE_DT &gt;5 and today() - CREATE_DT &lt;= 10 ,'6-10 Days',
-// //     if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &gt; 5 ,'Greater than 5 Days'))) as AgeBucket
-//     //'Primary' as Primary,
-//    // 'Van Request' As VanRequest
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\CDCKeyAccount\ParowOrderMan.qvd]
-// (qvd);
-// MyDays:
-// NoConcatenate
-// load distinct NumDate as DDate2
-// resident Data2
-// where wildmatch(STATUS,'Released','Allocated','In Progress','Picked');
-// Data3:
-// NoConcatenate
-// load * resident Data2
-// where exists(DDate2, NumDate);
-// drop table Data2;
-// drop table MyDays;
-// concatenate(Data)
-// LOAD * resident Data3;
-// drop table Data3;
-// Data2:
-// NoConcatenate
-// LOAD
-//     DDATE as DDATE,
-// //    date(date#(left(RPROUTE,8),'YYYYMMDD'),'YYYY/MM/DD') as DDATE,
-//     Num(date#(left(RPROUTE,8),'YYYYMMDD')) as NumDateP,
-//     num(Date#(DDATE, 'DD-MMM-YYYY')) as NumDate,
-//     right(RPROUTE,6) as ROUTEID,
-//     STATUS,
-//     ORDER_ID,
-//     "Customer ID" as CUST_ID,
-// //    SHIP_DOCK,
-//     SKU_ID as ITEM_ID,
-//     QTYORDERED,
-// //     RPROUTE,
-// //     QTYTASKED,
-// //     QTYPICKED,
-// //     PALLETSPICKED,
-// //     PALLETSOUT,
-// //     FULFILLED,
-// //     RATIO_1_TO_2,
-// //     Plant,
-//      CustomerName as CustomerNameVR
-// //     if(Left(ORDER_ID,2) = 'SO','SO', if(Left(ORDER_ID,2) = 'VQ','VQ',if(Left(ORDER_ID,2) = 'IF','IF'))) as Bucket,
-// //       if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &lt;= 2 ,'0-2 Days', 
-// //     if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &gt;2 and today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &lt;= 5 ,'3-5 Days',
-// //     //if(today() - CREATE_DT &gt;5 and today() - CREATE_DT &lt;= 10 ,'6-10 Days',
-// //     if(today()-Num(Date#(DDATE, 'DD-MMM-YYYY')) &gt; 5 ,'Greater than 5 Days'))) as AgeBucket
-//     //'Primary' as Primary,
-//    // 'Van Request' As VanRequest
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\CDCKeyAccount\PinetownOrderMan.qvd]
-// (qvd);
-// MyDays:
-// NoConcatenate
-// load distinct NumDate as DDate2
-// resident Data2
-// where wildmatch(STATUS,'Released','Allocated','In Progress','Picked');
-// Data3:
-// NoConcatenate
-// load * resident Data2
-// where exists(DDate2, NumDate);
-// drop table Data2;
-// drop table MyDays;
-// concatenate(Data)
-// LOAD * resident Data3;
-// drop table Data3;
-// Facttmp:
-// Noconcatenate
-// LOAD
-//  //   DDATEOld,
-//  NumDate+2 as TRANS_DATE,
-// //    date(NumDate,'YYYY/MM/DD') as DDATE,
-//     date(NumDate+if(weekday(NumDate)=4,3,2),'YYYY/MM/DD') as DelDATE,
-//     WeekDay(NumDate+if(weekday(NumDate)=4,3,if(weekday(NumDate)=3,4,2))) as CalDelDATE,
-//     NumDate,
-//     NumDateP,
-//     NumDateP-NumDate as DaysToPick,
-// //    Year(NumDate) as Year,
-// //    Month(NumDate) as Month,
-// //    left(RPROUTE,6) as YearMonth,
-// //    num(Week(NumDate)) as Week,
-// //    Year(NumDate)&amp;if(num(Week(NumDate))&lt;10,'0')&amp;num(Week(NumDate)) as YearWeek,
-// //    WeekDay(NumDate) as CalDay,
-// //    ROUTEID,
-//     STATUS as CDCSTATUS,
-//     ORDER_ID as CDCORDER_ID,
-//     num("CUST_ID")as CUST_ID,
-// //    SHIP_DOCK,
-//     num(ITEM_ID) as ITEM_ID,
-//     QTYORDERED,
-// //     QTYTASKED,
-// //     QTYPICKED,
-// //     RPROUTE,
-// //     PALLETSPICKED,
-// //     PALLETSOUT,
-// //     FULFILLED,
-// //     RATIO_1_TO_2,
-// //     Plant,
-// //     Bucket,
-// //    // if(Left(ORDER_ID,2) = 'SO','KA', if(Left(ORDER_ID,2) = 'VR','VR','IF')) as Category,
-// //    //  'Primary' as Primary,
-// //     // 'Van Request' As VanRequest
-//    CustomerNameVR
-// //   AgeBucket
-// resident Data
-// where left(ROUTEID,3)&lt;&gt;'EXP';
-// //where (WEEK1+("Shelf Life"/7))-Week(Today())&gt;0 and (WEEK1+("Shelf Life"/7))-Week(Today())&lt;=10;
-// drop table Data;
-///$tab Section
-// InvoicedQty:
-// LOAD
-//     upper(so_no) as CDCORDER_ID,
-//     INV_NO,
-//     INV_QTY
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\CDCKeyAccount\InvoicedQty.qvd]
-// (qvd);
-// LeadDays:
-// NoConcatenate
-// LOAD
-//     ADDRESS_ID as CustomerNameVR,
-// //    USER_DEF_TYPE_2 as CustomerType,
-//     if(USER_DEF_TYPE_2='DC',1,
-//      if(USER_DEF_TYPE_2='BIN',2,0)) as LeadDays
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\CloseToExpiry\LeadDayByAddressAndType.qvd]
-// (qvd);
-// left join (Facttmp)
-// load * resident LeadDays;
-// drop table LeadDays;
-// Fact:
-// NoConcatenate
-// load *,
-// //num(date(NumDate+LeadDays)) as TRANS_DATE,  
-// upper(date(NumDate+LeadDays,'DD-MMM-YYYY')) as DeliveryDate,
-//       if(today()-Num(Date#(upper(date(NumDate+LeadDays,'DD-MMM-YYYY')), 'DD-MMM-YYYY')) &lt; 0 ,'Tomorrow', 
-//     if(today()-Num(Date#(upper(date(NumDate+LeadDays,'DD-MMM-YYYY')), 'DD-MMM-YYYY')) =0 ,'Today',
-//     //if(today() - CREATE_DT &gt;5 and today() - CREATE_DT &lt;= 10 ,'6-10 Days',
-//     if(today()-Num(Date#(upper(date(NumDate+LeadDays,'DD-MMM-YYYY')), 'DD-MMM-YYYY')) &gt;= 1 ,'Yesterday'))) as DeliveryDateAgeBucket,
-//      TRANS_DATE &amp; '-' &amp; CUST_ID&amp; '-' &amp; ITEM_ID &amp; '-' &amp;  CDCORDER_ID as OrderLink
-// resident Facttmp;
-// drop table Facttmp;
-// LinkTableCDC: 
-// NoConcatenate
-// load distinct TRANS_DATE,
-// CUST_ID,
-// ITEM_ID, 
-// //YearWeek,
-// //ORDER_ID,
-// OrderLink 
-// Resident Fact;
-// drop fields  TRANS_DATE,
-// CUST_ID,
-// ITEM_ID 
-// //ORDER_ID 
-// From Fact;
-// // left join (LinkTable)
-// // load * resident InvoicedQty;
-// drop table InvoicedQty;
-///$tab LinkTable
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>LinkTable</t>
-        </is>
-      </c>
-      <c r="C25" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct CUST_ID,
-ITEM_ID,
-TDate as TRANS_DATE,
-OpenOrderLink
-resident OpenOrders;
-drop fields CUST_ID, ITEM_ID, [Date(CREATE_DT)] , TDate from OpenOrders;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>LinkTable2</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct CUST_ID,
-ITEM_ID,
-TRANS_DATE,
-SalesLink
-resident QlikViewUpdate;
-  drop fields CUST_ID, ITEM_ID, TRANS_DATE from QlikViewUpdate;
-join (LinkTable)
-load * resident LinkTable2;
-drop table LinkTable2;
-join(LinkTable)
-load * resident LinkTableCWO;
-drop table LinkTableCWO;
-// join (LinkTable)
-// load * resident LinkTableCDC;
-// drop table LinkTableCDC;
-// LinkTable3:
-// NoConcatenate
-// load distinct EDI_CWO_CUST_ID as CUST_ID,
-// ITEM_ID,
-// EDI_CWO_Date as TRANS_DATE,
-// [%EDI_LINK]
-// resident "EDI and CWO";
-// drop field ITEM_ID from "EDI and CWO";
-// join (LinkTable)
-// load * resident LinkTable3;
-// drop table LinkTable3;
-//exit script;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>LinkTable4</t>
-        </is>
-      </c>
-      <c r="C27" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct CUST_ID,
-ITEM_ID,
-TRANS_DATE,
-MonthlyLink
-resident MonthlySales;
-  drop fields CUST_ID, ITEM_ID, TRANS_DATE from MonthlySales;
-join (LinkTable)
-load * resident LinkTable4;
-drop table LinkTable4;
-// LinkTable5:
-// NoConcatenate
-// load distinct CUST_ID,
-// ITEM_ID,
-// TRANS_DATE,
-// OrdersToDeliverLink
-// resident OrdersToDeliver;
-//   drop fields CUST_ID, ITEM_ID, TRANS_DATE from OrdersToDeliver;
-// join (LinkTable)
-// load * resident LinkTable5;
-// drop table LinkTable5;
-// SAPRoute:
-// NoConcatenate
-// LOAD distinct replace(replace(subfield([Customer - Customer Level 01 (Key)],'.',2),'[',''),']','') as KAM, 
-//      replace(replace(subfield([Route - Route Level 01 (Key)],'.',2),'[',''),']','') as OriginalSAPRoute
-// FROM
-// [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\ESDOV0001-ZE_ESDOV0001_C000_00001.QVD]
-// (qvd);
-// SAPRouteNo:
-// NoConcatenate
-// LOAD distinct SLSMAN_CD as SAPRoute, 
-//      USER_DEFINE3 As OriginalSAPRoute,
-//      USER_DEFINE2 As SAPDTSRegion,
-//      BU_CD
-// FROM
-// [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\MST_SLSMAN.qvd]
-// (qvd);
-// left join (SAPRoute)
-// load * resident SAPRouteNo;
-// drop table SAPRouteNo;
-// NewDTSRegions:
-// NoConcatenate
-// LOAD
-//     REF_PARAM as BU_CD,
-//     REF_VALUE as SAP_ROUTE_LOCATION
-// FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/QVD\MasterData\SET_REF.qvd]
-// (qvd);
-// left join (SAPRoute)
-// load * resident NewDTSRegions;
-// drop table NewDTSRegions;
-// left join (RouteCustomerDetails)
-// load * resident SAPRoute;
-// drop table SAPRoute;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>RC</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct CUST_ID,
-//KAM,
-SAP_ROUTE_LOCATION, 
-//DTS_REGION,
-SAPDTSRegion
-resident RouteCustomerDetails;
-left join (LinkTable)
-load * resident RC;
-drop table RC; 
-//drop field ROUTE_LOCATION, DTS_REGION from RouteCustomerDetails;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>DCMap</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-LOAD distinct 
-    DC as SAP_ROUTE_LOCATION,
-    "DC MAP" as [DC MAP]
-FROM [lib://QSData (cwwpvt_qlikviewdev3) (cwwpvt_zaqlickviewadmin)/Excel/Daily Sales Report/DC MAP - Daily Sales.xlsx]
-(ooxml, embedded labels, table is Sheet1);
-left join (LinkTable)
-load * resident DCMap;
-left join (JDALink)
-load * resident DCMap;
-drop table DCMap; 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>RC</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load distinct SAP_ROUTE_LOCATION, 
-//DTS_REGION
-SAPDTSRegion
-resident RouteCustomerDetails;
-left join (JDALink)
-load * resident RC;
-drop table RC; 
-drop field SAP_ROUTE_LOCATION, SAPDTSRegion from RouteCustomerDetails;
-join (LinkTable)
-load * resident JDALink;
-drop table JDALink;  
-///$tab Calendar
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>Calendar</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOAD Distinct TRANS_DATE,
-	TRANS_DATE as TRANSE_DATE2,
-	year(TRANS_DATE) AS YEAR, 
-//	qvQUARTER AS QUARTER, 
-//	qvPERIOD AS PERIOD, 
-	month(TRANS_DATE) AS MONTH,
-    num(month(TRANS_DATE)) as MONTHNO,
-	week(TRANS_DATE) AS WEEK,
-    weekday(TRANS_DATE) As WEEKDAY,
-    date(TRANS_DATE,'YYYYMM') as YEARMONTH,
-    num(year(TRANS_DATE)&amp;if(week(TRANS_DATE)&lt;10,'0')&amp;week(TRANS_DATE)) as YEARWEEK, 
-//	WEEK(TRANS_DATE1) as WEEK,
-	text(date(TRANS_DATE,'YYYY/MM/DD')) as TRANS_DATE_LINK
-RESIDENT 
-	LinkTable;
-//     Calendar:
-//     load *,
-//     num(date#(TRANS_DATE2)) as TRANS_DATE
-//     resident Tmp;
-//     drop table Tmp;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Tmp</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOAD Ltrim(Rtrim(Upper(MAJOR_GROUP))) as MAJOR_GROUP, 
-     CATEGORY
-FROM
-[$(vFilePath2)/Category vs major grp mapping.xls]
-(biff, embedded labels, table is [New Mapping$]);
-//------------------------------------------------------------------------------------------------
-left join (RouteCustomerDetails)
-load * 
-,'Domestic' as INTER_COMPANY
-resident 
-	Tmp;
-drop table Tmp;
-//------------------------------------------------------------------------------------------------
-// Left Join (RouteCustomerDetails)
-// LOAD CUST_ID,
-// 	IF(CUST_ID = '419524' or CUST_ID = '428140', 'Exports', 'Domestic') AS INTER_COMPANY
-// Resident 
-// 	RouteCustomerDetails;
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>Tmp</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate
-load * resident RouteCustomerDetails
-where not WildMatch(CUST_ID,419524,428140);
-drop table RouteCustomerDetails;
-rename table Tmp to RouteCustomerDetails;
-///$tab Route Comms
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>RouteComms</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-LIB CONNECT TO '196.6.3.40 (NewsPage) (cwwpvt_zaqlickviewadmin)';
-LOAD "ROUTE_COUNT",
-    COMMUNICATED,
-    Perc;
-SQL SELECT "ROUTE_COUNT",
-    COMMUNICATED,
-    Perc
-FROM "SIMBA_DMS_LIVE".dbo."vQlikSense_RouteComms";
-///$tab Public Holiday
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>TMP</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOAD 
-PublicHolidays
-FROM
-[$(vFilePath)/PublicHolidays.xlsx]
-(ooxml, embedded labels, table is Sheet1);
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="inlineStr">
-        <is>
-          <t>Daily Sales Dashboard(1)</t>
-        </is>
-      </c>
-      <c r="B36" s="2" t="inlineStr">
-        <is>
-          <t>PublicHolidays</t>
-        </is>
-      </c>
-      <c r="C36" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NoConcatenate load
-*,
-MakeDate(right(PublicHolidays,4),mid(PublicHolidays,4,2),left(PublicHolidays,2)) as PubDate
-resident TMP;
-drop table TMP;
-///$tab exit script
-exit script;
-</t>
+          <t>NA</t>
         </is>
       </c>
     </row>

</xml_diff>